<commit_message>
fixato copertura progettazione 2
</commit_message>
<xml_diff>
--- a/input/generated_test_cases3_label_rimosse_feedbackAI_requisiti.xlsx
+++ b/input/generated_test_cases3_label_rimosse_feedbackAI_requisiti.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK285"/>
+  <dimension ref="A1:AK282"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13207,12 +13207,12 @@
     <row r="274">
       <c r="A274" s="2" t="inlineStr">
         <is>
-          <t>Carosello Home Page 1234 requisito-Carosello HP - TEST - Desktop_AIproposal_requisiti</t>
+          <t>Carosello Home Page 001 requisito-Carosello Home Page - TEST - Desktop_AIproposal_requisiti</t>
         </is>
       </c>
       <c r="B274" s="2" t="inlineStr">
         <is>
-          <t>TC-1234-01</t>
+          <t>CHP-001</t>
         </is>
       </c>
       <c r="C274" s="2" t="inlineStr"/>
@@ -13238,17 +13238,17 @@
       </c>
       <c r="H274" s="2" t="inlineStr">
         <is>
-          <t>UAT</t>
+          <t>TEST</t>
         </is>
       </c>
       <c r="I274" s="2" t="inlineStr">
         <is>
-          <t>Carosello Home Page</t>
+          <t>Windows 10, Chrome</t>
         </is>
       </c>
       <c r="J274" s="2" t="inlineStr">
         <is>
-          <t>Utente registrato e autenticato. Carosello configurato e attivo in Home Page.</t>
+          <t>Utente autenticato e Home Page accessibile.</t>
         </is>
       </c>
       <c r="K274" s="2" t="inlineStr">
@@ -13258,7 +13258,7 @@
       </c>
       <c r="L274" s="2" t="inlineStr">
         <is>
-          <t>Visualizzazione e navigazione del carosello in Home Page</t>
+          <t>Visualizzazione Carosello Home Page</t>
         </is>
       </c>
       <c r="M274" s="2" t="inlineStr">
@@ -13274,12 +13274,12 @@
       </c>
       <c r="P274" s="2" t="inlineStr">
         <is>
-          <t>Credenziali utente valide, dati di configurazione carosello attivi.</t>
+          <t>Account utente valido</t>
         </is>
       </c>
       <c r="Q274" s="2" t="inlineStr">
         <is>
-          <t>Il carosello viene visualizzato correttamente in Home Page, ogni card rispetta la struttura prevista e la navigazione tra le card è fluida.</t>
+          <t>Il carosello viene visualizzato correttamente nella Home Page con le card precompilate secondo le condizioni specificate.</t>
         </is>
       </c>
       <c r="R274" s="2" t="n">
@@ -13287,12 +13287,12 @@
       </c>
       <c r="S274" s="2" t="inlineStr">
         <is>
-          <t>Accedere all'applicativo tramite browser desktop e autenticarsi con credenziali valide.</t>
+          <t>Accedere alla Home Page dell'applicativo tramite browser desktop.</t>
         </is>
       </c>
       <c r="T274" s="2" t="inlineStr">
         <is>
-          <t>L'utente viene autenticato e viene visualizzata la Home Page.</t>
+          <t>La Home Page viene caricata correttamente.</t>
         </is>
       </c>
       <c r="U274" s="2" t="inlineStr">
@@ -13305,7 +13305,7 @@
       <c r="X274" s="2" t="inlineStr"/>
       <c r="Y274" s="2" t="inlineStr">
         <is>
-          <t>Test Scenario</t>
+          <t xml:space="preserve">Test </t>
         </is>
       </c>
       <c r="Z274" s="2" t="inlineStr"/>
@@ -13397,12 +13397,12 @@
       </c>
       <c r="S276" s="2" t="inlineStr">
         <is>
-          <t>Verificare che ogni card del carosello sia strutturata secondo le specifiche (precompilata, layout, contenuti).</t>
+          <t>Verificare che il carosello mostri le card precompilate secondo le condizioni di visualizzazione definite.</t>
         </is>
       </c>
       <c r="T276" s="2" t="inlineStr">
         <is>
-          <t>Ogni card del carosello rispetta la struttura predefinita e mostra i dati corretti.</t>
+          <t>Le card precompilate sono visualizzate correttamente nel carosello.</t>
         </is>
       </c>
       <c r="U276" s="2" t="inlineStr"/>
@@ -13424,43 +13424,115 @@
       <c r="AK276" s="2" t="inlineStr"/>
     </row>
     <row r="277">
-      <c r="A277" s="2" t="inlineStr"/>
-      <c r="B277" s="2" t="inlineStr"/>
+      <c r="A277" s="2" t="inlineStr">
+        <is>
+          <t>Carosello Home Page 002 requisito-Carosello Home Page - TEST - Mobile_android_AIproposal_requisiti</t>
+        </is>
+      </c>
+      <c r="B277" s="2" t="inlineStr">
+        <is>
+          <t>CHP-002</t>
+        </is>
+      </c>
       <c r="C277" s="2" t="inlineStr"/>
-      <c r="D277" s="2" t="inlineStr"/>
-      <c r="E277" s="2" t="inlineStr"/>
-      <c r="F277" s="2" t="inlineStr"/>
-      <c r="G277" s="2" t="inlineStr"/>
-      <c r="H277" s="2" t="inlineStr"/>
-      <c r="I277" s="2" t="inlineStr"/>
-      <c r="J277" s="2" t="inlineStr"/>
-      <c r="K277" s="2" t="inlineStr"/>
-      <c r="L277" s="2" t="inlineStr"/>
-      <c r="M277" s="2" t="inlineStr"/>
-      <c r="N277" s="2" t="inlineStr"/>
-      <c r="O277" s="2" t="inlineStr"/>
-      <c r="P277" s="2" t="inlineStr"/>
-      <c r="Q277" s="2" t="inlineStr"/>
+      <c r="D277" s="2" t="inlineStr">
+        <is>
+          <t>Mobile Android</t>
+        </is>
+      </c>
+      <c r="E277" s="2" t="inlineStr">
+        <is>
+          <t>Mobile</t>
+        </is>
+      </c>
+      <c r="F277" s="2" t="inlineStr">
+        <is>
+          <t>Smartphone</t>
+        </is>
+      </c>
+      <c r="G277" s="2" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="H277" s="2" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="I277" s="2" t="inlineStr">
+        <is>
+          <t>Android 12, App</t>
+        </is>
+      </c>
+      <c r="J277" s="2" t="inlineStr">
+        <is>
+          <t>Utente autenticato e Home Page accessibile.</t>
+        </is>
+      </c>
+      <c r="K277" s="2" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="L277" s="2" t="inlineStr">
+        <is>
+          <t>Visualizzazione Carosello Home Page su Android</t>
+        </is>
+      </c>
+      <c r="M277" s="2" t="inlineStr">
+        <is>
+          <t>functional</t>
+        </is>
+      </c>
+      <c r="N277" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O277" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="P277" s="2" t="inlineStr">
+        <is>
+          <t>Account utente valido</t>
+        </is>
+      </c>
+      <c r="Q277" s="2" t="inlineStr">
+        <is>
+          <t>Il carosello viene visualizzato e può essere navigato correttamente su dispositivi Android.</t>
+        </is>
+      </c>
       <c r="R277" s="2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S277" s="2" t="inlineStr">
         <is>
-          <t>Navigare tra le card del carosello utilizzando i controlli di navigazione (freccia destra/sinistra o swipe).</t>
+          <t>Aprire l'applicazione su dispositivo mobile Android.</t>
         </is>
       </c>
       <c r="T277" s="2" t="inlineStr">
         <is>
-          <t>La navigazione tra le card avviene senza errori e le card vengono caricate correttamente.</t>
-        </is>
-      </c>
-      <c r="U277" s="2" t="inlineStr"/>
+          <t>L'applicazione si avvia correttamente e mostra la Home Page.</t>
+        </is>
+      </c>
+      <c r="U277" s="2" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
       <c r="V277" s="2" t="inlineStr"/>
       <c r="W277" s="2" t="inlineStr"/>
       <c r="X277" s="2" t="inlineStr"/>
-      <c r="Y277" s="2" t="inlineStr"/>
+      <c r="Y277" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Test </t>
+        </is>
+      </c>
       <c r="Z277" s="2" t="inlineStr"/>
-      <c r="AA277" s="2" t="inlineStr"/>
+      <c r="AA277" s="2" t="inlineStr">
+        <is>
+          <t>sommario</t>
+        </is>
+      </c>
       <c r="AB277" s="2" t="inlineStr"/>
       <c r="AC277" s="2" t="inlineStr"/>
       <c r="AD277" s="2" t="inlineStr"/>
@@ -13473,115 +13545,43 @@
       <c r="AK277" s="2" t="inlineStr"/>
     </row>
     <row r="278">
-      <c r="A278" s="2" t="inlineStr">
-        <is>
-          <t>Carosello Home Page 1234 requisito-Carosello HP - TEST - Mobile_android_AIproposal_requisiti</t>
-        </is>
-      </c>
-      <c r="B278" s="2" t="inlineStr">
-        <is>
-          <t>TC-1234-02</t>
-        </is>
-      </c>
+      <c r="A278" s="2" t="inlineStr"/>
+      <c r="B278" s="2" t="inlineStr"/>
       <c r="C278" s="2" t="inlineStr"/>
-      <c r="D278" s="2" t="inlineStr">
-        <is>
-          <t>Mobile Android</t>
-        </is>
-      </c>
-      <c r="E278" s="2" t="inlineStr">
-        <is>
-          <t>Mobile</t>
-        </is>
-      </c>
-      <c r="F278" s="2" t="inlineStr">
-        <is>
-          <t>Smartphone</t>
-        </is>
-      </c>
-      <c r="G278" s="2" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="H278" s="2" t="inlineStr">
-        <is>
-          <t>UAT</t>
-        </is>
-      </c>
-      <c r="I278" s="2" t="inlineStr">
-        <is>
-          <t>Carosello Home Page</t>
-        </is>
-      </c>
-      <c r="J278" s="2" t="inlineStr">
-        <is>
-          <t>Utente registrato e autenticato. Carosello configurato e attivo in Home Page.</t>
-        </is>
-      </c>
-      <c r="K278" s="2" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
-      <c r="L278" s="2" t="inlineStr">
-        <is>
-          <t>Visualizzazione e navigazione del carosello in Home Page su Android</t>
-        </is>
-      </c>
-      <c r="M278" s="2" t="inlineStr">
-        <is>
-          <t>functional</t>
-        </is>
-      </c>
-      <c r="N278" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="O278" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="P278" s="2" t="inlineStr">
-        <is>
-          <t>Credenziali utente valide, dati di configurazione carosello attivi.</t>
-        </is>
-      </c>
-      <c r="Q278" s="2" t="inlineStr">
-        <is>
-          <t>Il carosello viene visualizzato correttamente in Home Page su Android, ogni card rispetta la struttura prevista e la navigazione tra le card è fluida.</t>
-        </is>
-      </c>
+      <c r="D278" s="2" t="inlineStr"/>
+      <c r="E278" s="2" t="inlineStr"/>
+      <c r="F278" s="2" t="inlineStr"/>
+      <c r="G278" s="2" t="inlineStr"/>
+      <c r="H278" s="2" t="inlineStr"/>
+      <c r="I278" s="2" t="inlineStr"/>
+      <c r="J278" s="2" t="inlineStr"/>
+      <c r="K278" s="2" t="inlineStr"/>
+      <c r="L278" s="2" t="inlineStr"/>
+      <c r="M278" s="2" t="inlineStr"/>
+      <c r="N278" s="2" t="inlineStr"/>
+      <c r="O278" s="2" t="inlineStr"/>
+      <c r="P278" s="2" t="inlineStr"/>
+      <c r="Q278" s="2" t="inlineStr"/>
       <c r="R278" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S278" s="2" t="inlineStr">
         <is>
-          <t>Aprire l'applicazione mobile su dispositivo Android e autenticarsi con credenziali valide.</t>
+          <t>Verificare la presenza del carosello nella Home Page.</t>
         </is>
       </c>
       <c r="T278" s="2" t="inlineStr">
         <is>
-          <t>L'utente viene autenticato e viene visualizzata la Home Page.</t>
-        </is>
-      </c>
-      <c r="U278" s="2" t="inlineStr">
-        <is>
-          <t>Italy</t>
-        </is>
-      </c>
+          <t>Il carosello è visibile nella posizione prevista della Home Page.</t>
+        </is>
+      </c>
+      <c r="U278" s="2" t="inlineStr"/>
       <c r="V278" s="2" t="inlineStr"/>
       <c r="W278" s="2" t="inlineStr"/>
       <c r="X278" s="2" t="inlineStr"/>
-      <c r="Y278" s="2" t="inlineStr">
-        <is>
-          <t>Test Scenario</t>
-        </is>
-      </c>
+      <c r="Y278" s="2" t="inlineStr"/>
       <c r="Z278" s="2" t="inlineStr"/>
-      <c r="AA278" s="2" t="inlineStr">
-        <is>
-          <t>sommario</t>
-        </is>
-      </c>
+      <c r="AA278" s="2" t="inlineStr"/>
       <c r="AB278" s="2" t="inlineStr"/>
       <c r="AC278" s="2" t="inlineStr"/>
       <c r="AD278" s="2" t="inlineStr"/>
@@ -13612,16 +13612,16 @@
       <c r="P279" s="2" t="inlineStr"/>
       <c r="Q279" s="2" t="inlineStr"/>
       <c r="R279" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S279" s="2" t="inlineStr">
         <is>
-          <t>Verificare la presenza del carosello nella Home Page.</t>
+          <t>Scorrere il carosello orizzontalmente.</t>
         </is>
       </c>
       <c r="T279" s="2" t="inlineStr">
         <is>
-          <t>Il carosello è visibile nella posizione prevista della Home Page.</t>
+          <t>Le card precompilate scorrono fluidamente e sono visualizzate correttamente.</t>
         </is>
       </c>
       <c r="U279" s="2" t="inlineStr"/>
@@ -13643,43 +13643,115 @@
       <c r="AK279" s="2" t="inlineStr"/>
     </row>
     <row r="280">
-      <c r="A280" s="2" t="inlineStr"/>
-      <c r="B280" s="2" t="inlineStr"/>
+      <c r="A280" s="2" t="inlineStr">
+        <is>
+          <t>Carosello Home Page 003 requisito-Carosello Home Page - TEST - Mobile_ios_AIproposal_requisiti</t>
+        </is>
+      </c>
+      <c r="B280" s="2" t="inlineStr">
+        <is>
+          <t>CHP-003</t>
+        </is>
+      </c>
       <c r="C280" s="2" t="inlineStr"/>
-      <c r="D280" s="2" t="inlineStr"/>
-      <c r="E280" s="2" t="inlineStr"/>
-      <c r="F280" s="2" t="inlineStr"/>
-      <c r="G280" s="2" t="inlineStr"/>
-      <c r="H280" s="2" t="inlineStr"/>
-      <c r="I280" s="2" t="inlineStr"/>
-      <c r="J280" s="2" t="inlineStr"/>
-      <c r="K280" s="2" t="inlineStr"/>
-      <c r="L280" s="2" t="inlineStr"/>
-      <c r="M280" s="2" t="inlineStr"/>
-      <c r="N280" s="2" t="inlineStr"/>
-      <c r="O280" s="2" t="inlineStr"/>
-      <c r="P280" s="2" t="inlineStr"/>
-      <c r="Q280" s="2" t="inlineStr"/>
+      <c r="D280" s="2" t="inlineStr">
+        <is>
+          <t>Mobile IOS</t>
+        </is>
+      </c>
+      <c r="E280" s="2" t="inlineStr">
+        <is>
+          <t>Mobile</t>
+        </is>
+      </c>
+      <c r="F280" s="2" t="inlineStr">
+        <is>
+          <t>Smartphone</t>
+        </is>
+      </c>
+      <c r="G280" s="2" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="H280" s="2" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="I280" s="2" t="inlineStr">
+        <is>
+          <t>iOS 16, App</t>
+        </is>
+      </c>
+      <c r="J280" s="2" t="inlineStr">
+        <is>
+          <t>Utente autenticato e Home Page accessibile.</t>
+        </is>
+      </c>
+      <c r="K280" s="2" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="L280" s="2" t="inlineStr">
+        <is>
+          <t>Visualizzazione Carosello Home Page su iOS</t>
+        </is>
+      </c>
+      <c r="M280" s="2" t="inlineStr">
+        <is>
+          <t>functional</t>
+        </is>
+      </c>
+      <c r="N280" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O280" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="P280" s="2" t="inlineStr">
+        <is>
+          <t>Account utente valido</t>
+        </is>
+      </c>
+      <c r="Q280" s="2" t="inlineStr">
+        <is>
+          <t>Il carosello viene visualizzato e può essere navigato correttamente su dispositivi iOS.</t>
+        </is>
+      </c>
       <c r="R280" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="S280" s="2" t="inlineStr">
         <is>
-          <t>Verificare che ogni card del carosello sia strutturata secondo le specifiche (precompilata, layout, contenuti).</t>
+          <t>Aprire l'applicazione su dispositivo mobile iOS.</t>
         </is>
       </c>
       <c r="T280" s="2" t="inlineStr">
         <is>
-          <t>Ogni card del carosello rispetta la struttura predefinita e mostra i dati corretti.</t>
-        </is>
-      </c>
-      <c r="U280" s="2" t="inlineStr"/>
+          <t>L'applicazione si avvia correttamente e mostra la Home Page.</t>
+        </is>
+      </c>
+      <c r="U280" s="2" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
       <c r="V280" s="2" t="inlineStr"/>
       <c r="W280" s="2" t="inlineStr"/>
       <c r="X280" s="2" t="inlineStr"/>
-      <c r="Y280" s="2" t="inlineStr"/>
+      <c r="Y280" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Test </t>
+        </is>
+      </c>
       <c r="Z280" s="2" t="inlineStr"/>
-      <c r="AA280" s="2" t="inlineStr"/>
+      <c r="AA280" s="2" t="inlineStr">
+        <is>
+          <t>sommario</t>
+        </is>
+      </c>
       <c r="AB280" s="2" t="inlineStr"/>
       <c r="AC280" s="2" t="inlineStr"/>
       <c r="AD280" s="2" t="inlineStr"/>
@@ -13710,16 +13782,16 @@
       <c r="P281" s="2" t="inlineStr"/>
       <c r="Q281" s="2" t="inlineStr"/>
       <c r="R281" s="2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S281" s="2" t="inlineStr">
         <is>
-          <t>Navigare tra le card del carosello effettuando swipe a destra e sinistra.</t>
+          <t>Verificare la presenza del carosello nella Home Page.</t>
         </is>
       </c>
       <c r="T281" s="2" t="inlineStr">
         <is>
-          <t>La navigazione tra le card avviene senza errori e le card vengono caricate correttamente.</t>
+          <t>Il carosello è visibile nella posizione prevista della Home Page.</t>
         </is>
       </c>
       <c r="U281" s="2" t="inlineStr"/>
@@ -13741,115 +13813,43 @@
       <c r="AK281" s="2" t="inlineStr"/>
     </row>
     <row r="282">
-      <c r="A282" s="2" t="inlineStr">
-        <is>
-          <t>Carosello Home Page 1234 requisito-Carosello HP - TEST - Mobile_ios_AIproposal_requisiti</t>
-        </is>
-      </c>
-      <c r="B282" s="2" t="inlineStr">
-        <is>
-          <t>TC-1234-03</t>
-        </is>
-      </c>
+      <c r="A282" s="2" t="inlineStr"/>
+      <c r="B282" s="2" t="inlineStr"/>
       <c r="C282" s="2" t="inlineStr"/>
-      <c r="D282" s="2" t="inlineStr">
-        <is>
-          <t>Mobile IOS</t>
-        </is>
-      </c>
-      <c r="E282" s="2" t="inlineStr">
-        <is>
-          <t>Mobile</t>
-        </is>
-      </c>
-      <c r="F282" s="2" t="inlineStr">
-        <is>
-          <t>Smartphone</t>
-        </is>
-      </c>
-      <c r="G282" s="2" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="H282" s="2" t="inlineStr">
-        <is>
-          <t>UAT</t>
-        </is>
-      </c>
-      <c r="I282" s="2" t="inlineStr">
-        <is>
-          <t>Carosello Home Page</t>
-        </is>
-      </c>
-      <c r="J282" s="2" t="inlineStr">
-        <is>
-          <t>Utente registrato e autenticato. Carosello configurato e attivo in Home Page.</t>
-        </is>
-      </c>
-      <c r="K282" s="2" t="inlineStr">
-        <is>
-          <t>Manual</t>
-        </is>
-      </c>
-      <c r="L282" s="2" t="inlineStr">
-        <is>
-          <t>Visualizzazione e navigazione del carosello in Home Page su iOS</t>
-        </is>
-      </c>
-      <c r="M282" s="2" t="inlineStr">
-        <is>
-          <t>functional</t>
-        </is>
-      </c>
-      <c r="N282" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="O282" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="P282" s="2" t="inlineStr">
-        <is>
-          <t>Credenziali utente valide, dati di configurazione carosello attivi.</t>
-        </is>
-      </c>
-      <c r="Q282" s="2" t="inlineStr">
-        <is>
-          <t>Il carosello viene visualizzato correttamente in Home Page su iOS, ogni card rispetta la struttura prevista e la navigazione tra le card è fluida.</t>
-        </is>
-      </c>
+      <c r="D282" s="2" t="inlineStr"/>
+      <c r="E282" s="2" t="inlineStr"/>
+      <c r="F282" s="2" t="inlineStr"/>
+      <c r="G282" s="2" t="inlineStr"/>
+      <c r="H282" s="2" t="inlineStr"/>
+      <c r="I282" s="2" t="inlineStr"/>
+      <c r="J282" s="2" t="inlineStr"/>
+      <c r="K282" s="2" t="inlineStr"/>
+      <c r="L282" s="2" t="inlineStr"/>
+      <c r="M282" s="2" t="inlineStr"/>
+      <c r="N282" s="2" t="inlineStr"/>
+      <c r="O282" s="2" t="inlineStr"/>
+      <c r="P282" s="2" t="inlineStr"/>
+      <c r="Q282" s="2" t="inlineStr"/>
       <c r="R282" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S282" s="2" t="inlineStr">
         <is>
-          <t>Aprire l'applicazione mobile su dispositivo iOS e autenticarsi con credenziali valide.</t>
+          <t>Scorrere il carosello orizzontalmente.</t>
         </is>
       </c>
       <c r="T282" s="2" t="inlineStr">
         <is>
-          <t>L'utente viene autenticato e viene visualizzata la Home Page.</t>
-        </is>
-      </c>
-      <c r="U282" s="2" t="inlineStr">
-        <is>
-          <t>Italy</t>
-        </is>
-      </c>
+          <t>Le card precompilate scorrono fluidamente e sono visualizzate correttamente.</t>
+        </is>
+      </c>
+      <c r="U282" s="2" t="inlineStr"/>
       <c r="V282" s="2" t="inlineStr"/>
       <c r="W282" s="2" t="inlineStr"/>
       <c r="X282" s="2" t="inlineStr"/>
-      <c r="Y282" s="2" t="inlineStr">
-        <is>
-          <t>Test Scenario</t>
-        </is>
-      </c>
+      <c r="Y282" s="2" t="inlineStr"/>
       <c r="Z282" s="2" t="inlineStr"/>
-      <c r="AA282" s="2" t="inlineStr">
-        <is>
-          <t>sommario</t>
-        </is>
-      </c>
+      <c r="AA282" s="2" t="inlineStr"/>
       <c r="AB282" s="2" t="inlineStr"/>
       <c r="AC282" s="2" t="inlineStr"/>
       <c r="AD282" s="2" t="inlineStr"/>
@@ -13861,153 +13861,6 @@
       <c r="AJ282" s="2" t="inlineStr"/>
       <c r="AK282" s="2" t="inlineStr"/>
     </row>
-    <row r="283">
-      <c r="A283" s="2" t="inlineStr"/>
-      <c r="B283" s="2" t="inlineStr"/>
-      <c r="C283" s="2" t="inlineStr"/>
-      <c r="D283" s="2" t="inlineStr"/>
-      <c r="E283" s="2" t="inlineStr"/>
-      <c r="F283" s="2" t="inlineStr"/>
-      <c r="G283" s="2" t="inlineStr"/>
-      <c r="H283" s="2" t="inlineStr"/>
-      <c r="I283" s="2" t="inlineStr"/>
-      <c r="J283" s="2" t="inlineStr"/>
-      <c r="K283" s="2" t="inlineStr"/>
-      <c r="L283" s="2" t="inlineStr"/>
-      <c r="M283" s="2" t="inlineStr"/>
-      <c r="N283" s="2" t="inlineStr"/>
-      <c r="O283" s="2" t="inlineStr"/>
-      <c r="P283" s="2" t="inlineStr"/>
-      <c r="Q283" s="2" t="inlineStr"/>
-      <c r="R283" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="S283" s="2" t="inlineStr">
-        <is>
-          <t>Verificare la presenza del carosello nella Home Page.</t>
-        </is>
-      </c>
-      <c r="T283" s="2" t="inlineStr">
-        <is>
-          <t>Il carosello è visibile nella posizione prevista della Home Page.</t>
-        </is>
-      </c>
-      <c r="U283" s="2" t="inlineStr"/>
-      <c r="V283" s="2" t="inlineStr"/>
-      <c r="W283" s="2" t="inlineStr"/>
-      <c r="X283" s="2" t="inlineStr"/>
-      <c r="Y283" s="2" t="inlineStr"/>
-      <c r="Z283" s="2" t="inlineStr"/>
-      <c r="AA283" s="2" t="inlineStr"/>
-      <c r="AB283" s="2" t="inlineStr"/>
-      <c r="AC283" s="2" t="inlineStr"/>
-      <c r="AD283" s="2" t="inlineStr"/>
-      <c r="AE283" s="2" t="inlineStr"/>
-      <c r="AF283" s="2" t="inlineStr"/>
-      <c r="AG283" s="2" t="inlineStr"/>
-      <c r="AH283" s="2" t="inlineStr"/>
-      <c r="AI283" s="2" t="inlineStr"/>
-      <c r="AJ283" s="2" t="inlineStr"/>
-      <c r="AK283" s="2" t="inlineStr"/>
-    </row>
-    <row r="284">
-      <c r="A284" s="2" t="inlineStr"/>
-      <c r="B284" s="2" t="inlineStr"/>
-      <c r="C284" s="2" t="inlineStr"/>
-      <c r="D284" s="2" t="inlineStr"/>
-      <c r="E284" s="2" t="inlineStr"/>
-      <c r="F284" s="2" t="inlineStr"/>
-      <c r="G284" s="2" t="inlineStr"/>
-      <c r="H284" s="2" t="inlineStr"/>
-      <c r="I284" s="2" t="inlineStr"/>
-      <c r="J284" s="2" t="inlineStr"/>
-      <c r="K284" s="2" t="inlineStr"/>
-      <c r="L284" s="2" t="inlineStr"/>
-      <c r="M284" s="2" t="inlineStr"/>
-      <c r="N284" s="2" t="inlineStr"/>
-      <c r="O284" s="2" t="inlineStr"/>
-      <c r="P284" s="2" t="inlineStr"/>
-      <c r="Q284" s="2" t="inlineStr"/>
-      <c r="R284" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="S284" s="2" t="inlineStr">
-        <is>
-          <t>Verificare che ogni card del carosello sia strutturata secondo le specifiche (precompilata, layout, contenuti).</t>
-        </is>
-      </c>
-      <c r="T284" s="2" t="inlineStr">
-        <is>
-          <t>Ogni card del carosello rispetta la struttura predefinita e mostra i dati corretti.</t>
-        </is>
-      </c>
-      <c r="U284" s="2" t="inlineStr"/>
-      <c r="V284" s="2" t="inlineStr"/>
-      <c r="W284" s="2" t="inlineStr"/>
-      <c r="X284" s="2" t="inlineStr"/>
-      <c r="Y284" s="2" t="inlineStr"/>
-      <c r="Z284" s="2" t="inlineStr"/>
-      <c r="AA284" s="2" t="inlineStr"/>
-      <c r="AB284" s="2" t="inlineStr"/>
-      <c r="AC284" s="2" t="inlineStr"/>
-      <c r="AD284" s="2" t="inlineStr"/>
-      <c r="AE284" s="2" t="inlineStr"/>
-      <c r="AF284" s="2" t="inlineStr"/>
-      <c r="AG284" s="2" t="inlineStr"/>
-      <c r="AH284" s="2" t="inlineStr"/>
-      <c r="AI284" s="2" t="inlineStr"/>
-      <c r="AJ284" s="2" t="inlineStr"/>
-      <c r="AK284" s="2" t="inlineStr"/>
-    </row>
-    <row r="285">
-      <c r="A285" s="2" t="inlineStr"/>
-      <c r="B285" s="2" t="inlineStr"/>
-      <c r="C285" s="2" t="inlineStr"/>
-      <c r="D285" s="2" t="inlineStr"/>
-      <c r="E285" s="2" t="inlineStr"/>
-      <c r="F285" s="2" t="inlineStr"/>
-      <c r="G285" s="2" t="inlineStr"/>
-      <c r="H285" s="2" t="inlineStr"/>
-      <c r="I285" s="2" t="inlineStr"/>
-      <c r="J285" s="2" t="inlineStr"/>
-      <c r="K285" s="2" t="inlineStr"/>
-      <c r="L285" s="2" t="inlineStr"/>
-      <c r="M285" s="2" t="inlineStr"/>
-      <c r="N285" s="2" t="inlineStr"/>
-      <c r="O285" s="2" t="inlineStr"/>
-      <c r="P285" s="2" t="inlineStr"/>
-      <c r="Q285" s="2" t="inlineStr"/>
-      <c r="R285" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="S285" s="2" t="inlineStr">
-        <is>
-          <t>Navigare tra le card del carosello effettuando swipe a destra e sinistra.</t>
-        </is>
-      </c>
-      <c r="T285" s="2" t="inlineStr">
-        <is>
-          <t>La navigazione tra le card avviene senza errori e le card vengono caricate correttamente.</t>
-        </is>
-      </c>
-      <c r="U285" s="2" t="inlineStr"/>
-      <c r="V285" s="2" t="inlineStr"/>
-      <c r="W285" s="2" t="inlineStr"/>
-      <c r="X285" s="2" t="inlineStr"/>
-      <c r="Y285" s="2" t="inlineStr"/>
-      <c r="Z285" s="2" t="inlineStr"/>
-      <c r="AA285" s="2" t="inlineStr"/>
-      <c r="AB285" s="2" t="inlineStr"/>
-      <c r="AC285" s="2" t="inlineStr"/>
-      <c r="AD285" s="2" t="inlineStr"/>
-      <c r="AE285" s="2" t="inlineStr"/>
-      <c r="AF285" s="2" t="inlineStr"/>
-      <c r="AG285" s="2" t="inlineStr"/>
-      <c r="AH285" s="2" t="inlineStr"/>
-      <c r="AI285" s="2" t="inlineStr"/>
-      <c r="AJ285" s="2" t="inlineStr"/>
-      <c r="AK285" s="2" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>